<commit_message>
đã thành công,trước khi thêm cột score_i
</commit_message>
<xml_diff>
--- a/public/upload/file_mau/bang_tong_hop_danh_gia_ren_luyen.xlsx
+++ b/public/upload/file_mau/bang_tong_hop_danh_gia_ren_luyen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Laravel\luanvantotnghiep\upload\file_mau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Laravel\luanvantotnghiep\public\upload\file_mau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -403,7 +403,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -637,59 +637,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -793,54 +745,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,62 +766,68 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -931,17 +841,11 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1272,43 +1176,43 @@
       <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="I2" s="67" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="I2" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
       <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -1326,34 +1230,34 @@
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
     </row>
     <row r="7" spans="1:15" s="3" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
@@ -1374,84 +1278,84 @@
     <row r="8" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="71" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
     </row>
     <row r="9" spans="1:15" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72" t="s">
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
     </row>
     <row r="10" spans="1:15" s="3" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="63" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59" t="s">
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="59" t="s">
+      <c r="K11" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="59" t="s">
+      <c r="L11" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="59" t="s">
+      <c r="N11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="59" t="s">
+      <c r="O11" s="43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="64"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="10" t="s">
         <v>11</v>
       </c>
@@ -1461,13 +1365,13 @@
       <c r="H12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
     </row>
     <row r="13" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
@@ -1476,10 +1380,10 @@
       <c r="B13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="66"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="24" t="s">
         <v>21</v>
       </c>
@@ -1648,48 +1552,48 @@
       <c r="O20" s="14"/>
     </row>
     <row r="22" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
-      <c r="F22" s="61" t="s">
+      <c r="F22" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61" t="s">
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="F23" s="60" t="s">
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="F23" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60" t="s">
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
     </row>
     <row r="24" spans="1:15" s="18" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E24" s="22"/>
@@ -1712,151 +1616,181 @@
       <c r="E28" s="22"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="62" t="s">
+      <c r="A29" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="62"/>
-      <c r="N29" s="62"/>
-      <c r="O29" s="62"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62"/>
-      <c r="O30" s="62"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
     </row>
     <row r="31" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="62"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="23"/>
-      <c r="G31" s="62" t="s">
+      <c r="G31" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="62"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="62"/>
-      <c r="L31" s="62" t="s">
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="L31" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="M31" s="62"/>
+      <c r="M31" s="55"/>
     </row>
     <row r="32" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="62"/>
+      <c r="C32" s="55"/>
       <c r="D32" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="23"/>
-      <c r="G32" s="62" t="s">
+      <c r="G32" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="62"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="62"/>
-      <c r="L32" s="62" t="s">
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="L32" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="M32" s="62"/>
+      <c r="M32" s="55"/>
     </row>
     <row r="33" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="62"/>
+      <c r="C33" s="55"/>
       <c r="D33" s="17" t="s">
         <v>40</v>
       </c>
       <c r="E33" s="23"/>
-      <c r="G33" s="62" t="s">
+      <c r="G33" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="L33" s="62" t="s">
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="L33" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="M33" s="62"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="60"/>
-      <c r="U33" s="60"/>
-      <c r="V33" s="60"/>
-      <c r="W33" s="60"/>
+      <c r="M33" s="55"/>
+      <c r="S33" s="54"/>
+      <c r="T33" s="54"/>
+      <c r="U33" s="54"/>
+      <c r="V33" s="54"/>
+      <c r="W33" s="54"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="62"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="62"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="60"/>
-      <c r="U34" s="60"/>
-      <c r="V34" s="60"/>
-      <c r="W34" s="60"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55"/>
+      <c r="S34" s="54"/>
+      <c r="T34" s="54"/>
+      <c r="U34" s="54"/>
+      <c r="V34" s="54"/>
+      <c r="W34" s="54"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="62"/>
-      <c r="N35" s="62"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="S34:U34"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A35:N35"/>
+    <mergeCell ref="A34:N34"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="L32:M32"/>
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="C11:D12"/>
     <mergeCell ref="I3:O3"/>
@@ -1873,36 +1807,6 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="N11:N12"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A35:N35"/>
-    <mergeCell ref="A34:N34"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="S34:U34"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="A30:O30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="S33:U33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.2" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -1915,7 +1819,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1936,43 +1840,43 @@
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:15" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="I2" s="67" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="I2" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:15" s="26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
       <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
     </row>
     <row r="4" spans="1:15" s="26" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -1983,41 +1887,41 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:15" s="56" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="84" t="s">
+    <row r="5" spans="1:15" s="40" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
     </row>
     <row r="6" spans="1:15" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
     </row>
     <row r="7" spans="1:15" s="26" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
@@ -2038,83 +1942,83 @@
     <row r="8" spans="1:15" s="26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="29"/>
       <c r="C8" s="5"/>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
     </row>
     <row r="9" spans="1:15" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="29"/>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72" t="s">
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
     </row>
     <row r="10" spans="1:15" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="29"/>
     </row>
     <row r="11" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="83" t="s">
+      <c r="D11" s="63"/>
+      <c r="E11" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="77" t="s">
+      <c r="F11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77" t="s">
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="77" t="s">
+      <c r="J11" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="77" t="s">
+      <c r="K11" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="77" t="s">
+      <c r="L11" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="77" t="s">
+      <c r="M11" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="77" t="s">
+      <c r="N11" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="79" t="s">
+      <c r="O11" s="65" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="82"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="64"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="10" t="s">
         <v>11</v>
       </c>
@@ -2124,223 +2028,94 @@
       <c r="H12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="80"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="76"/>
-      <c r="E13" s="53" t="s">
+      <c r="D13" s="68"/>
+      <c r="E13" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="52" t="s">
+      <c r="F13" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="52" t="s">
+      <c r="G13" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="52" t="s">
+      <c r="H13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="52" t="s">
+      <c r="I13" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="52" t="s">
+      <c r="J13" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="52" t="s">
+      <c r="K13" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="52" t="s">
+      <c r="L13" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="52" t="s">
+      <c r="M13" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="52" t="s">
+      <c r="N13" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="54" t="s">
+      <c r="O13" s="38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="50"/>
-    </row>
-    <row r="15" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="36"/>
-    </row>
-    <row r="16" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="36"/>
-    </row>
-    <row r="17" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="36"/>
-    </row>
-    <row r="18" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="36"/>
-    </row>
-    <row r="19" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="36"/>
-    </row>
-    <row r="20" spans="1:15" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="36"/>
-    </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="37"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
-    </row>
-    <row r="22" spans="1:15" ht="14.4" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="E8:M8"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="I3:O3"/>
     <mergeCell ref="A6:O6"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="E8:M8"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>